<commit_message>
Add Multi-processing capability in kick_off_tests method in Initiator class
</commit_message>
<xml_diff>
--- a/Tests/E2E_UW_02_PC_AC_01.xlsx
+++ b/Tests/E2E_UW_02_PC_AC_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\eclipse-workspace\GuidewireGenericFramework\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna.teja.taduri\PycharmProjects\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ED2B21-DAD0-4F74-BC36-0BA12C63E81B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A524CE-69CD-4FD8-9CD0-DBD3EB104E98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{783CBA7D-5567-428F-B69C-AE07AD0048B3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="92">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -66,9 +66,6 @@
     <t>LaunchBrowser</t>
   </si>
   <si>
-    <t>UrlTest</t>
-  </si>
-  <si>
     <t>Click</t>
   </si>
   <si>
@@ -153,15 +150,6 @@
     <t>Bosch</t>
   </si>
   <si>
-    <t>UrlST</t>
-  </si>
-  <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
     <t>m_Sample</t>
   </si>
   <si>
@@ -310,6 +298,15 @@
   </si>
   <si>
     <t>CloseBrowser</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>State: ON</t>
+  </si>
+  <si>
+    <t>PolicyCenter</t>
   </si>
 </sst>
 </file>
@@ -697,11 +694,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB727FA6-C75F-46B7-A1BB-752E1EB442DB}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,15 +742,15 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -767,19 +765,19 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -805,97 +803,97 @@
         <v>9</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>9</v>
@@ -907,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -915,19 +913,19 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>9</v>
@@ -939,7 +937,7 @@
         <v>9</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -947,19 +945,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>9</v>
@@ -971,7 +969,7 @@
         <v>9</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -979,31 +977,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1011,19 +1009,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>9</v>
@@ -1035,7 +1033,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1043,19 +1041,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>9</v>
@@ -1067,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1075,20 +1073,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="4">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1099,15 +1097,15 @@
         <v>9</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -1122,24 +1120,24 @@
         <v>5</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>9</v>
@@ -1151,51 +1149,51 @@
         <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1203,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>9</v>
@@ -1215,19 +1213,19 @@
         <v>9</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1235,31 +1233,31 @@
         <v>7</v>
       </c>
       <c r="B17" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1267,31 +1265,31 @@
         <v>7</v>
       </c>
       <c r="B18" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1299,31 +1297,31 @@
         <v>7</v>
       </c>
       <c r="B19" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1331,31 +1329,31 @@
         <v>7</v>
       </c>
       <c r="B20" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1363,31 +1361,31 @@
         <v>7</v>
       </c>
       <c r="B21" s="4">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="G21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1395,31 +1393,31 @@
         <v>7</v>
       </c>
       <c r="B22" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1427,19 +1425,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>9</v>
@@ -1451,7 +1449,7 @@
         <v>9</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1459,31 +1457,31 @@
         <v>7</v>
       </c>
       <c r="B24" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -1491,19 +1489,19 @@
         <v>7</v>
       </c>
       <c r="B25" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="F25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>9</v>
@@ -1515,7 +1513,7 @@
         <v>9</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1523,10 +1521,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>9</v>
@@ -1538,16 +1536,16 @@
         <v>5</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1555,31 +1553,31 @@
         <v>7</v>
       </c>
       <c r="B27" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="J27" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -1587,19 +1585,19 @@
         <v>7</v>
       </c>
       <c r="B28" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>9</v>
@@ -1611,7 +1609,7 @@
         <v>9</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -1619,7 +1617,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
@@ -1634,7 +1632,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>9</v>
@@ -1643,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -1651,7 +1649,7 @@
         <v>7</v>
       </c>
       <c r="B30" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>9</v>
@@ -1663,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>9</v>
@@ -1675,14 +1673,17 @@
         <v>9</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Duplicate Value" error="An object already exists with this name." sqref="D4:E5" xr:uid="{8BA74F7F-5338-4D8F-9E3D-2107F46C95A0}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" display="https://gwdisc.fslabs.io/pc/PolicyCenter.do" xr:uid="{4EB6F067-B594-4FB8-964B-F233B567D23B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>